<commit_message>
validacao de dados, mensagens de erro
</commit_message>
<xml_diff>
--- a/2.Excel/hands-on/5.Ferramentas_dados/4.Validação de Dados.xlsx
+++ b/2.Excel/hands-on/5.Ferramentas_dados/4.Validação de Dados.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaof\Desktop\Excel Impressionador 2021\Módulo 7 - Ferramentas de Dados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Projetos para Github\Hashtag\2.Excel\hands-on\5.Ferramentas_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C740BA-6949-4CBA-B312-CF1D59B75C7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D34E7122-1A72-4F28-ADD0-7AA22B51DF67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="1000" xr2:uid="{0D445F65-54A1-41E5-865A-2279466CCF1F}"/>
+    <workbookView xWindow="12180" yWindow="96" windowWidth="10896" windowHeight="12792" tabRatio="536" xr2:uid="{0D445F65-54A1-41E5-865A-2279466CCF1F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Base" sheetId="2" r:id="rId1"/>
-    <sheet name="Paises" sheetId="3" r:id="rId2"/>
-    <sheet name="Pratica" sheetId="4" r:id="rId3"/>
+    <sheet name="Aula 1" sheetId="5" r:id="rId1"/>
+    <sheet name="Base" sheetId="2" r:id="rId2"/>
+    <sheet name="Paises" sheetId="3" r:id="rId3"/>
+    <sheet name="Pratica" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Paises!$A$1:$E$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Paises!$A$1:$E$55</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="71">
   <si>
     <t>Nome</t>
   </si>
@@ -240,6 +241,18 @@
   </si>
   <si>
     <t>País</t>
+  </si>
+  <si>
+    <t>Leila Alecrim</t>
+  </si>
+  <si>
+    <t>Filipe Dourado</t>
+  </si>
+  <si>
+    <t>Cássia Henrique</t>
+  </si>
+  <si>
+    <t>Feminino</t>
   </si>
 </sst>
 </file>
@@ -324,21 +337,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -652,36 +663,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40D11AF4-2C8D-4548-9F11-4E03C4C35DE5}">
-  <dimension ref="A1:I7089"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90FAC829-2744-4A24-A395-A0899F934D89}">
+  <dimension ref="A1:H7089"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.5546875" customWidth="1"/>
     <col min="2" max="6" width="19.21875" customWidth="1"/>
     <col min="8" max="8" width="12.44140625" customWidth="1"/>
-    <col min="9" max="9" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="6" t="s">
         <v>9</v>
       </c>
       <c r="H1" s="3" t="s">
@@ -689,128 +701,324 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="10"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
+      <c r="A2" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="2">
+        <v>12345678901</v>
+      </c>
       <c r="H2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="11"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
+      <c r="A3" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
       <c r="H3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
+      <c r="A4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
       <c r="H4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
       <c r="H5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="7089" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7089" s="1"/>
+    </row>
+  </sheetData>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Informação inválida" error="Você precisa informar um dos seguintes valores: masculino, feminino ou outros." promptTitle="ATENÇÃO" prompt="Digite uma das opções: masculino, feminino ou outros." sqref="C2:C15" xr:uid="{B3B11EFD-2FB8-40E9-B55B-0855B749B597}">
+      <formula1>"Masculino,Feminino,Outros"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D15" xr:uid="{AE236DAA-F9FB-44BD-9A69-B91E43B5692B}">
+      <formula1>0</formula1>
+      <formula2>120</formula2>
+    </dataValidation>
+    <dataValidation type="date" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E15 E2" xr:uid="{069E66B1-39FB-439C-9C90-3027683B82A1}">
+      <formula1>42369</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F15" xr:uid="{86181083-DD66-41E6-BBDE-A2BC8FAA3AF0}">
+      <formula1>11</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40D11AF4-2C8D-4548-9F11-4E03C4C35DE5}">
+  <dimension ref="A1:H7089"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.5546875" customWidth="1"/>
+    <col min="2" max="6" width="19.21875" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="7"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="H2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="8"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="H3" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="H4" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="H5" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
     </row>
     <row r="7089" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7089" s="1"/>
@@ -821,9 +1029,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F53E3B8-6343-4ACB-9A1F-E8EA93C2EABE}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
@@ -833,297 +1041,198 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="A2" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" t="s">
         <v>59</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+      <c r="A4" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+      <c r="A5" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" t="s">
         <v>45</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
+      <c r="A6" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
+      <c r="A7" t="s">
         <v>56</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" t="s">
         <v>54</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
+      <c r="A8" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
+      <c r="A9" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
+      <c r="A10" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
+      <c r="A11" t="s">
         <v>64</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" t="s">
         <v>62</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" t="s">
         <v>61</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="4"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="4"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="4"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="4"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="4"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="4"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4078EFF-B788-452D-9850-73BA89964DF3}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1135,16 +1244,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
validacao de dados, continuacao
</commit_message>
<xml_diff>
--- a/2.Excel/hands-on/5.Ferramentas_dados/4.Validação de Dados.xlsx
+++ b/2.Excel/hands-on/5.Ferramentas_dados/4.Validação de Dados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Projetos para Github\Hashtag\2.Excel\hands-on\5.Ferramentas_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D34E7122-1A72-4F28-ADD0-7AA22B51DF67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E7EFD4D-E79A-471C-85D0-ACBD63717D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12180" yWindow="96" windowWidth="10896" windowHeight="12792" tabRatio="536" xr2:uid="{0D445F65-54A1-41E5-865A-2279466CCF1F}"/>
+    <workbookView xWindow="12144" yWindow="96" windowWidth="10896" windowHeight="12792" tabRatio="536" xr2:uid="{0D445F65-54A1-41E5-865A-2279466CCF1F}"/>
   </bookViews>
   <sheets>
     <sheet name="Aula 1" sheetId="5" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="73">
   <si>
     <t>Nome</t>
   </si>
@@ -253,14 +253,21 @@
   </si>
   <si>
     <t>Feminino</t>
+  </si>
+  <si>
+    <t>05123256984</t>
+  </si>
+  <si>
+    <t>Junior Caique</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="165" formatCode="000&quot;.&quot;000&quot;.&quot;000&quot;-&quot;00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -310,7 +317,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -333,11 +340,107 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -350,11 +453,193 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="10">
+    <dxf>
+      <numFmt numFmtId="165" formatCode="000&quot;.&quot;000&quot;.&quot;000&quot;-&quot;00"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -365,6 +650,21 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7E334D4B-6180-4F61-B93A-D84EB1A03C5C}" name="Tabela1" displayName="Tabela1" ref="A1:F17" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6">
+  <autoFilter ref="A1:F17" xr:uid="{7E334D4B-6180-4F61-B93A-D84EB1A03C5C}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{29B0C16F-1A65-44BE-A9F4-989FDF5082B9}" name="Nome" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{26B32CE2-A43B-477A-81C4-811B7A50067B}" name="Equipe" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{8666A9B8-47FC-41C4-8C88-B6B4FF0EF175}" name="Sexo" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{E71DCE32-BA96-4E95-80DD-4AF17CF90433}" name="Idade" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{582CC995-3C50-4E55-A3D4-C7969D5AEA20}" name="Nascimento" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{1620E580-AB6A-4BC3-8121-15EA6D95A32B}" name="CPF" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -666,8 +966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90FAC829-2744-4A24-A395-A0899F934D89}">
   <dimension ref="A1:H7089"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -678,22 +978,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="16" t="s">
         <v>9</v>
       </c>
       <c r="H1" s="3" t="s">
@@ -701,160 +1001,194 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="C2" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="2">
-        <v>12345678901</v>
+      <c r="D2" s="2">
+        <v>53</v>
+      </c>
+      <c r="E2" s="9">
+        <v>25624</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>71</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="11" t="s">
         <v>68</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="F3" s="13">
+        <v>12345678963</v>
+      </c>
       <c r="H3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="12" t="s">
         <v>69</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="F4" s="13"/>
       <c r="H4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="F5" s="13"/>
       <c r="H5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
+      <c r="A6" s="12"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="F6" s="13"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
+      <c r="A7" s="12"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="F7" s="13"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
+      <c r="A8" s="12"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="F8" s="13"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="F9" s="13"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="F10" s="13"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="F11" s="13"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
+      <c r="A12" s="12"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="F12" s="13"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
+      <c r="A13" s="12"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="F13" s="13"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
+      <c r="A14" s="12"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="F14" s="13"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+      <c r="A15" s="17"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="19"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="19"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="17"/>
+      <c r="B17" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="19"/>
     </row>
     <row r="7089" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7089" s="1"/>
     </row>
   </sheetData>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Informação inválida" error="Você precisa informar um dos seguintes valores: masculino, feminino ou outros." promptTitle="ATENÇÃO" prompt="Digite uma das opções: masculino, feminino ou outros." sqref="C2:C15" xr:uid="{B3B11EFD-2FB8-40E9-B55B-0855B749B597}">
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Informação inválida" error="Você precisa informar um dos seguintes valores: masculino, feminino ou outros." promptTitle="ATENÇÃO" prompt="Digite uma das opções: masculino, feminino ou outros." sqref="C2:C17" xr:uid="{B3B11EFD-2FB8-40E9-B55B-0855B749B597}">
       <formula1>"Masculino,Feminino,Outros"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D15" xr:uid="{AE236DAA-F9FB-44BD-9A69-B91E43B5692B}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D17" xr:uid="{AE236DAA-F9FB-44BD-9A69-B91E43B5692B}">
       <formula1>0</formula1>
       <formula2>120</formula2>
     </dataValidation>
-    <dataValidation type="date" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E15 E2" xr:uid="{069E66B1-39FB-439C-9C90-3027683B82A1}">
+    <dataValidation type="date" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E15" xr:uid="{069E66B1-39FB-439C-9C90-3027683B82A1}">
       <formula1>42369</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F15" xr:uid="{86181083-DD66-41E6-BBDE-A2BC8FAA3AF0}">
+    <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F17" xr:uid="{F36FBF9D-B3DA-4323-853E-31318B2BC5C8}">
       <formula1>11</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B17" xr:uid="{705450B1-2387-49DB-9DA1-290CE17032F0}">
+      <formula1>$H$2:$H$5</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
validacao de dado, intervalos nomeados
</commit_message>
<xml_diff>
--- a/2.Excel/hands-on/5.Ferramentas_dados/4.Validação de Dados.xlsx
+++ b/2.Excel/hands-on/5.Ferramentas_dados/4.Validação de Dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Projetos para Github\Hashtag\2.Excel\hands-on\5.Ferramentas_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E7EFD4D-E79A-471C-85D0-ACBD63717D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA2B1019-8FA1-4461-AC06-C51BF7C4F16D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12144" yWindow="96" windowWidth="10896" windowHeight="12792" tabRatio="536" xr2:uid="{0D445F65-54A1-41E5-865A-2279466CCF1F}"/>
   </bookViews>
@@ -20,6 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Paises!$A$1:$E$55</definedName>
+    <definedName name="Lista_equipes">'Aula 1'!$H$2:$H$5</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="73">
   <si>
     <t>Nome</t>
   </si>
@@ -584,6 +585,15 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -591,15 +601,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -653,7 +654,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7E334D4B-6180-4F61-B93A-D84EB1A03C5C}" name="Tabela1" displayName="Tabela1" ref="A1:F17" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7E334D4B-6180-4F61-B93A-D84EB1A03C5C}" name="Tabela1" displayName="Tabela1" ref="A1:F17" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <autoFilter ref="A1:F17" xr:uid="{7E334D4B-6180-4F61-B93A-D84EB1A03C5C}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{29B0C16F-1A65-44BE-A9F4-989FDF5082B9}" name="Nome" dataDxfId="5"/>
@@ -967,7 +968,7 @@
   <dimension ref="A1:H7089"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1004,9 +1005,7 @@
       <c r="A2" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
         <v>70</v>
       </c>
@@ -1154,9 +1153,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="17"/>
-      <c r="B17" s="18" t="s">
-        <v>2</v>
-      </c>
+      <c r="B17" s="18"/>
       <c r="C17" s="18"/>
       <c r="D17" s="18"/>
       <c r="E17" s="18"/>
@@ -1180,8 +1177,8 @@
     <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F17" xr:uid="{F36FBF9D-B3DA-4323-853E-31318B2BC5C8}">
       <formula1>11</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B17" xr:uid="{705450B1-2387-49DB-9DA1-290CE17032F0}">
-      <formula1>$H$2:$H$5</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B17" xr:uid="{49A72EC7-0F2B-4128-A565-CC38B3EF7869}">
+      <formula1>Lista_equipes</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
validacao dados, lista condicionada
</commit_message>
<xml_diff>
--- a/2.Excel/hands-on/5.Ferramentas_dados/4.Validação de Dados.xlsx
+++ b/2.Excel/hands-on/5.Ferramentas_dados/4.Validação de Dados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Projetos para Github\Hashtag\2.Excel\hands-on\5.Ferramentas_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA2B1019-8FA1-4461-AC06-C51BF7C4F16D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E61D7E-262C-4585-917D-2B1052BEAB3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12144" yWindow="96" windowWidth="10896" windowHeight="12792" tabRatio="536" xr2:uid="{0D445F65-54A1-41E5-865A-2279466CCF1F}"/>
+    <workbookView xWindow="12144" yWindow="96" windowWidth="10896" windowHeight="12792" tabRatio="536" firstSheet="1" activeTab="3" xr2:uid="{0D445F65-54A1-41E5-865A-2279466CCF1F}"/>
   </bookViews>
   <sheets>
     <sheet name="Aula 1" sheetId="5" r:id="rId1"/>
@@ -20,7 +20,12 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Paises!$A$1:$E$55</definedName>
+    <definedName name="África">Paises!$A$2:$A$11</definedName>
+    <definedName name="América">Paises!$B$2:$B$11</definedName>
+    <definedName name="Ásia">Paises!$C$2:$C$11</definedName>
+    <definedName name="Europa">Paises!$D$2:$D$12</definedName>
     <definedName name="Lista_equipes">'Aula 1'!$H$2:$H$5</definedName>
+    <definedName name="Oceania">Paises!$E$2:$E$11</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,8 +45,43 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Filipe Cayres</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{90C17233-CFCA-46EE-A102-65772E4E51A4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Filipe Cayres:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+a fórmula INDIRETO() é utilizada para puxarmos o intervalo nomeado que está na célula. 
+OBS: o intervalo precisa ter o nome exatamente igual ao do valor oferecido na célula</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="74">
   <si>
     <t>Nome</t>
   </si>
@@ -260,6 +300,9 @@
   </si>
   <si>
     <t>Junior Caique</t>
+  </si>
+  <si>
+    <t>Espanha</t>
   </si>
 </sst>
 </file>
@@ -270,7 +313,7 @@
     <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
     <numFmt numFmtId="165" formatCode="000&quot;.&quot;000&quot;.&quot;000&quot;-&quot;00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -284,6 +327,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -470,7 +526,127 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2" tint="-0.749992370372631"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2" tint="-0.749992370372631"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2" tint="-0.749992370372631"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2" tint="-0.749992370372631"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2" tint="-0.749992370372631"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="000&quot;.&quot;000&quot;.&quot;000&quot;-&quot;00"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -654,17 +830,67 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7E334D4B-6180-4F61-B93A-D84EB1A03C5C}" name="Tabela1" displayName="Tabela1" ref="A1:F17" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7E334D4B-6180-4F61-B93A-D84EB1A03C5C}" name="Tabela1" displayName="Tabela1" ref="A1:F17" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <autoFilter ref="A1:F17" xr:uid="{7E334D4B-6180-4F61-B93A-D84EB1A03C5C}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{29B0C16F-1A65-44BE-A9F4-989FDF5082B9}" name="Nome" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{26B32CE2-A43B-477A-81C4-811B7A50067B}" name="Equipe" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{8666A9B8-47FC-41C4-8C88-B6B4FF0EF175}" name="Sexo" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{E71DCE32-BA96-4E95-80DD-4AF17CF90433}" name="Idade" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{582CC995-3C50-4E55-A3D4-C7969D5AEA20}" name="Nascimento" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{1620E580-AB6A-4BC3-8121-15EA6D95A32B}" name="CPF" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{29B0C16F-1A65-44BE-A9F4-989FDF5082B9}" name="Nome" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{26B32CE2-A43B-477A-81C4-811B7A50067B}" name="Equipe" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{8666A9B8-47FC-41C4-8C88-B6B4FF0EF175}" name="Sexo" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{E71DCE32-BA96-4E95-80DD-4AF17CF90433}" name="Idade" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{582CC995-3C50-4E55-A3D4-C7969D5AEA20}" name="Nascimento" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{1620E580-AB6A-4BC3-8121-15EA6D95A32B}" name="CPF" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{53881F72-3828-4DC4-AF33-018B6A88B9BA}" name="Tabela2" displayName="Tabela2" ref="A1:A11" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:A11" xr:uid="{53881F72-3828-4DC4-AF33-018B6A88B9BA}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{8D21C4C0-6AD0-4EED-8A86-C10F3E7BF940}" name="África"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D91C791A-4D18-46D9-9D24-FA5B4F2ABF7F}" name="Tabela3" displayName="Tabela3" ref="B1:B11" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="B1:B11" xr:uid="{D91C791A-4D18-46D9-9D24-FA5B4F2ABF7F}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{015C55CF-4252-4714-9F67-DD72830A8E20}" name="América"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{24C3BB23-1BD2-4BC8-B4C3-748DF94AE9A2}" name="Tabela4" displayName="Tabela4" ref="C1:C11" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="C1:C11" xr:uid="{24C3BB23-1BD2-4BC8-B4C3-748DF94AE9A2}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{588DCC38-D9F0-4EBE-91C3-A15EE4C87CED}" name="Ásia"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{020EC094-15DF-4FE5-AA43-6EC091EBF732}" name="Tabela5" displayName="Tabela5" ref="D1:D12" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="D1:D12" xr:uid="{020EC094-15DF-4FE5-AA43-6EC091EBF732}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{60B38FAE-9A15-4740-8E51-39EBCC4E1A2D}" name="Europa"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{1846F7BD-0E60-4F0A-AF1A-34CB1B910841}" name="Tabela6" displayName="Tabela6" ref="E1:E11" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="E1:E11" xr:uid="{1846F7BD-0E60-4F0A-AF1A-34CB1B910841}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{65E828F5-063F-4BC9-B44F-C1FB902BE6C6}" name="Oceania"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -967,7 +1193,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90FAC829-2744-4A24-A395-A0899F934D89}">
   <dimension ref="A1:H7089"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
@@ -1362,9 +1588,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F53E3B8-6343-4ACB-9A1F-E8EA93C2EABE}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1558,16 +1786,30 @@
         <v>35</v>
       </c>
     </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>73</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <tableParts count="5">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4078EFF-B788-452D-9850-73BA89964DF3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4078EFF-B788-452D-9850-73BA89964DF3}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1583,10 +1825,30 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
+      <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="B2" s="2"/>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{7B256847-E578-413A-A57D-A0A89EC3D8DB}">
+      <formula1>INDIRECT(A2)</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6C519D56-77C8-4481-B652-E99D68AA0C99}">
+          <x14:formula1>
+            <xm:f>Paises!$A$1:$E$1</xm:f>
+          </x14:formula1>
+          <xm:sqref>A2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
validacao de dados, avisos e informacoes
</commit_message>
<xml_diff>
--- a/2.Excel/hands-on/5.Ferramentas_dados/4.Validação de Dados.xlsx
+++ b/2.Excel/hands-on/5.Ferramentas_dados/4.Validação de Dados.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Projetos para Github\Hashtag\2.Excel\hands-on\5.Ferramentas_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E61D7E-262C-4585-917D-2B1052BEAB3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7AF4BEE-D56F-4C5E-B6CE-04DE83FC3957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12144" yWindow="96" windowWidth="10896" windowHeight="12792" tabRatio="536" firstSheet="1" activeTab="3" xr2:uid="{0D445F65-54A1-41E5-865A-2279466CCF1F}"/>
+    <workbookView xWindow="12144" yWindow="96" windowWidth="10896" windowHeight="12792" tabRatio="536" activeTab="1" xr2:uid="{0D445F65-54A1-41E5-865A-2279466CCF1F}"/>
   </bookViews>
   <sheets>
     <sheet name="Aula 1" sheetId="5" r:id="rId1"/>
-    <sheet name="Base" sheetId="2" r:id="rId2"/>
-    <sheet name="Paises" sheetId="3" r:id="rId3"/>
-    <sheet name="Pratica" sheetId="4" r:id="rId4"/>
+    <sheet name="Aula2" sheetId="6" r:id="rId2"/>
+    <sheet name="Base" sheetId="2" r:id="rId3"/>
+    <sheet name="Paises" sheetId="3" r:id="rId4"/>
+    <sheet name="Pratica" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Paises!$A$1:$E$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Paises!$A$1:$E$55</definedName>
     <definedName name="África">Paises!$A$2:$A$11</definedName>
     <definedName name="América">Paises!$B$2:$B$11</definedName>
     <definedName name="Ásia">Paises!$C$2:$C$11</definedName>
@@ -81,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="75">
   <si>
     <t>Nome</t>
   </si>
@@ -303,6 +304,9 @@
   </si>
   <si>
     <t>Espanha</t>
+  </si>
+  <si>
+    <t>Black</t>
   </si>
 </sst>
 </file>
@@ -1416,11 +1420,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40D11AF4-2C8D-4548-9F11-4E03C4C35DE5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CF38C7E-D1E6-4770-94F4-EA12F00E0F78}">
   <dimension ref="A1:H7089"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1455,6 +1459,210 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="7"/>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="H2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="8"/>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="H3" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="H4" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="H5" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="7089" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7089" s="1"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B15" xr:uid="{986E1AA1-028C-402D-A6D4-69A65E7207E1}">
+      <formula1>$H$2:$H$5</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40D11AF4-2C8D-4548-9F11-4E03C4C35DE5}">
+  <dimension ref="A1:H7089"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.5546875" customWidth="1"/>
+    <col min="2" max="6" width="19.21875" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="7"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -1586,7 +1794,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F53E3B8-6343-4ACB-9A1F-E8EA93C2EABE}">
   <dimension ref="A1:E12"/>
   <sheetViews>
@@ -1803,11 +2011,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4078EFF-B788-452D-9850-73BA89964DF3}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>